<commit_message>
Finalizare schemă + adăugare footprint pentru majoritatea componentelor
</commit_message>
<xml_diff>
--- a/Calcule/Calcule.xlsx
+++ b/Calcule/Calcule.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="2145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="2145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Comutarea LED-urilor" sheetId="1" r:id="rId1"/>
     <sheet name="Comutarea 7 segmentului" sheetId="2" r:id="rId2"/>
+    <sheet name="Comutarea buzzer-ului" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="85">
   <si>
     <t>Comutarea LED-urilor</t>
   </si>
@@ -818,6 +819,46 @@
   <si>
     <t>Amplificarea în curent a tranzistorului 2.</t>
   </si>
+  <si>
+    <t>Comutarea buzzer-ului</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>EBsat</t>
+    </r>
+  </si>
+  <si>
+    <t>Tensiunea E-B când tranzistorul este în saturație.</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>BUZZ</t>
+    </r>
+  </si>
+  <si>
+    <t>Curentul prin buzzer.</t>
+  </si>
+  <si>
+    <t>kΩ</t>
+  </si>
 </sst>
 </file>
 
@@ -1322,6 +1363,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,7 +1408,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1378,45 +1458,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2507,8 +2548,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1173335" cy="372346"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -2727,7 +2768,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -3444,8 +3485,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2336345" cy="344582"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -3695,7 +3736,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -3802,8 +3843,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="992644" cy="184089"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -4010,7 +4051,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -4153,8 +4194,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="634404" cy="316946"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -4299,7 +4340,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -4394,8 +4435,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="865365" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -4602,7 +4643,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -4733,8 +4774,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1280479" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -4978,7 +5019,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -5130,8 +5171,8 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2367123" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -5531,7 +5572,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -5698,8 +5739,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="605422" cy="372346"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -5760,7 +5801,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -5872,7 +5913,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -6023,8 +6064,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="634404" cy="316946"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -6169,7 +6210,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -6264,8 +6305,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="865365" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12"/>
@@ -6472,7 +6513,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12"/>
@@ -6603,8 +6644,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1026114" cy="190886"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13"/>
@@ -6805,7 +6846,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13"/>
@@ -6936,8 +6977,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1280479" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14"/>
@@ -7181,7 +7222,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14"/>
@@ -7333,8 +7374,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2367123" cy="365549"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15"/>
@@ -7728,7 +7769,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15"/>
@@ -7895,8 +7936,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="608692" cy="372346"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16"/>
@@ -7957,7 +7998,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -8069,7 +8110,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16"/>
@@ -8174,6 +8215,1792 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="876522" cy="184089"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1495425" y="6915150"/>
+              <a:ext cx="876522" cy="184089"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐵</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1495425" y="6915150"/>
+              <a:ext cx="876522" cy="184089"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=𝐼_(𝐵_2 )+𝐼_𝐵</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="664284" cy="316946"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1495425" y="6105525"/>
+              <a:ext cx="664284" cy="316946"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐵</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐼</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵𝑈𝑍𝑍</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>10</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1495425" y="6105525"/>
+              <a:ext cx="664284" cy="316946"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵=𝐼_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵𝑈𝑍𝑍</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/10</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="758221" cy="365549"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1504950" y="6496050"/>
+              <a:ext cx="758221" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐸𝐵</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑠𝑎𝑡</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝐵</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1504950" y="6496050"/>
+              <a:ext cx="758221" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=𝑉_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠𝑎𝑡/𝑅_(𝐵_2 ) </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1173335" cy="365549"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1514475" y="7191375"/>
+              <a:ext cx="1173335" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐶𝐶</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐸𝐵</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑠𝑎𝑡</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐼</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝐵</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1514475" y="7191375"/>
+              <a:ext cx="1173335" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=(𝑉_𝐶𝐶−𝑉_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠𝑎𝑡)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼_(𝐵_1 ) </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2180084" cy="365549"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9182100" y="6057900"/>
+              <a:ext cx="2180084" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐵</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐶𝐶</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵𝐸𝑠𝑎𝑡</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝐵</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9182100" y="6057900"/>
+              <a:ext cx="2180084" cy="365549"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐼</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵=𝐼_(𝐵_1 )−𝐼_(𝐵_2 )=(𝑉_𝐶𝐶−𝑉_𝐵𝐸𝑠𝑎𝑡)/𝑅_(𝐵_1 ) −𝐼_(𝐵_2 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="618952" cy="344582"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9239250" y="6391275"/>
+              <a:ext cx="618952" cy="344582"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="el-GR" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>β</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐼</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵𝑈𝑍𝑍</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐼</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ro-RO" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9239250" y="6391275"/>
+              <a:ext cx="618952" cy="344582"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>β</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=𝐼_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵𝑈𝑍𝑍</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ro-RO" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/𝐼_𝐵 </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>168669</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>39703</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10848975" y="863994"/>
+          <a:ext cx="2286000" cy="3014284"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8443,7 +10270,7 @@
   <dimension ref="B2:P48"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8463,53 +10290,53 @@
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:16" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="26"/>
-      <c r="D8" s="28"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="8" t="s">
         <v>4</v>
       </c>
@@ -8519,7 +10346,7 @@
       <c r="G8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
@@ -8609,34 +10436,34 @@
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="26"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="8" t="s">
         <v>4</v>
       </c>
@@ -8646,7 +10473,7 @@
       <c r="G17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
@@ -8710,56 +10537,56 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="J23" s="47" t="s">
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
+      <c r="J23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="49"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="34"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="K24" s="27" t="s">
+      <c r="K24" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="29" t="s">
+      <c r="L24" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="30" t="s">
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="26"/>
-      <c r="D25" s="28"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="8" t="s">
         <v>4</v>
       </c>
@@ -8769,9 +10596,9 @@
       <c r="G25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="31"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="28"/>
+      <c r="H25" s="44"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="39"/>
       <c r="L25" s="8" t="s">
         <v>4</v>
       </c>
@@ -8781,7 +10608,7 @@
       <c r="N25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O25" s="31"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" s="15" t="s">
@@ -8965,100 +10792,100 @@
     </row>
     <row r="32" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
-      <c r="J33" s="32" t="s">
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="47"/>
+      <c r="J33" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="34"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="47"/>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="35"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="37"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="50"/>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="38"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="40"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="53"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="38"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="40"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="53"/>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C37" s="38"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="40"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="53"/>
     </row>
     <row r="38" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="38"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="43"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="53"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="56"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="38"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
       <c r="L39" s="22"/>
@@ -9067,12 +10894,12 @@
       <c r="O39" s="22"/>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="38"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
@@ -9081,12 +10908,12 @@
       <c r="O40" s="21"/>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="38"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="40"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="53"/>
       <c r="J41" s="21"/>
       <c r="K41" s="21"/>
       <c r="L41" s="21"/>
@@ -9095,12 +10922,12 @@
       <c r="O41" s="21"/>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="38"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="53"/>
       <c r="J42" s="21"/>
       <c r="K42" s="21"/>
       <c r="L42" s="21"/>
@@ -9109,12 +10936,12 @@
       <c r="O42" s="21"/>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="38"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="53"/>
       <c r="J43" s="21"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
@@ -9123,12 +10950,12 @@
       <c r="O43" s="21"/>
     </row>
     <row r="44" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="43"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="56"/>
       <c r="J44" s="21"/>
       <c r="K44" s="21"/>
       <c r="L44" s="21"/>
@@ -9194,19 +11021,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="D3:N3"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C6:H6"/>
     <mergeCell ref="J34:O38"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
@@ -9219,6 +11033,19 @@
     <mergeCell ref="L24:N24"/>
     <mergeCell ref="O24:O25"/>
     <mergeCell ref="J33:O33"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9230,8 +11057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9251,53 +11078,53 @@
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:16" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="46"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="26"/>
-      <c r="D8" s="28"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="8" t="s">
         <v>4</v>
       </c>
@@ -9307,7 +11134,7 @@
       <c r="G8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
@@ -9396,10 +11223,10 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="26" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="9">
@@ -9413,7 +11240,7 @@
         <f>F13+8/100*F13</f>
         <v>10.8</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="27" t="s">
         <v>30</v>
       </c>
     </row>
@@ -9441,34 +11268,34 @@
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="30" t="s">
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="26"/>
-      <c r="D19" s="28"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="8" t="s">
         <v>4</v>
       </c>
@@ -9478,7 +11305,7 @@
       <c r="G19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
@@ -9541,22 +11368,22 @@
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="26">
         <v>40</v>
       </c>
-      <c r="F23" s="51">
+      <c r="F23" s="26">
         <v>100</v>
       </c>
-      <c r="G23" s="51">
+      <c r="G23" s="26">
         <v>180</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -9582,56 +11409,56 @@
     </row>
     <row r="26" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
-      <c r="J27" s="47" t="s">
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
+      <c r="J27" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="49"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="34"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30" t="s">
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="L28" s="29" t="s">
+      <c r="L28" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="30" t="s">
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="26"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="8" t="s">
         <v>4</v>
       </c>
@@ -9641,9 +11468,9 @@
       <c r="G29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="31"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="28"/>
+      <c r="H29" s="44"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="39"/>
       <c r="L29" s="8" t="s">
         <v>4</v>
       </c>
@@ -9653,7 +11480,7 @@
       <c r="N29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O29" s="31"/>
+      <c r="O29" s="44"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" s="15" t="s">
@@ -9721,25 +11548,25 @@
       <c r="H31" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J31" s="53" t="s">
+      <c r="J31" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="K31" s="54" t="s">
+      <c r="K31" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="55">
+      <c r="L31" s="30">
         <f>E30/N30</f>
         <v>0.14907615991334833</v>
       </c>
-      <c r="M31" s="55">
+      <c r="M31" s="30">
         <f>F30/M30</f>
         <v>2.0469850015304552</v>
       </c>
-      <c r="N31" s="55">
+      <c r="N31" s="30">
         <f>G30/L30</f>
         <v>9.7256079433973479</v>
       </c>
-      <c r="O31" s="56" t="s">
+      <c r="O31" s="31" t="s">
         <v>44</v>
       </c>
     </row>
@@ -9954,142 +11781,142 @@
     </row>
     <row r="39" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="J40" s="32" t="s">
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="47"/>
+      <c r="J40" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="34"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="47"/>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="37"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="50"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="50"/>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="38"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="40"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="53"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="53"/>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="38"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="40"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="53"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="53"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="38"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="40"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="53"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="53"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="38"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="40"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="53"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="53"/>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="38"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="40"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="40"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="53"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="53"/>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C47" s="38"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="40"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="53"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="53"/>
     </row>
     <row r="48" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="38"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
-      <c r="O48" s="43"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="53"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="55"/>
+      <c r="N48" s="55"/>
+      <c r="O48" s="56"/>
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C49" s="38"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="53"/>
       <c r="J49" s="22"/>
       <c r="K49" s="22"/>
       <c r="L49" s="22"/>
@@ -10098,12 +11925,12 @@
       <c r="O49" s="22"/>
     </row>
     <row r="50" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C50" s="38"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="53"/>
       <c r="J50" s="21"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
@@ -10112,12 +11939,12 @@
       <c r="O50" s="21"/>
     </row>
     <row r="51" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="38"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="53"/>
       <c r="J51" s="21"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
@@ -10126,12 +11953,12 @@
       <c r="O51" s="21"/>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="38"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="53"/>
       <c r="J52" s="21"/>
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
@@ -10140,12 +11967,12 @@
       <c r="O52" s="21"/>
     </row>
     <row r="53" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="38"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="53"/>
       <c r="J53" s="21"/>
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
@@ -10154,12 +11981,12 @@
       <c r="O53" s="21"/>
     </row>
     <row r="54" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C54" s="38"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="53"/>
       <c r="J54" s="21"/>
       <c r="K54" s="21"/>
       <c r="L54" s="21"/>
@@ -10168,12 +11995,12 @@
       <c r="O54" s="21"/>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="38"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="53"/>
       <c r="J55" s="21"/>
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
@@ -10182,12 +12009,12 @@
       <c r="O55" s="21"/>
     </row>
     <row r="56" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C56" s="38"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="53"/>
       <c r="J56" s="21"/>
       <c r="K56" s="21"/>
       <c r="L56" s="21"/>
@@ -10196,12 +12023,12 @@
       <c r="O56" s="21"/>
     </row>
     <row r="57" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="38"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="53"/>
       <c r="J57" s="21"/>
       <c r="K57" s="21"/>
       <c r="L57" s="21"/>
@@ -10210,12 +12037,12 @@
       <c r="O57" s="21"/>
     </row>
     <row r="58" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="41"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="43"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="56"/>
       <c r="J58" s="21"/>
       <c r="K58" s="21"/>
       <c r="L58" s="21"/>
@@ -10281,6 +12108,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:H19"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="J40:O40"/>
     <mergeCell ref="C41:H58"/>
@@ -10294,12 +12132,690 @@
     <mergeCell ref="K28:K29"/>
     <mergeCell ref="L28:N28"/>
     <mergeCell ref="O28:O29"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:H19"/>
     <mergeCell ref="C27:H27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:16" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="44"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3.3</v>
+      </c>
+      <c r="G9" s="16">
+        <v>5.5</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9">
+        <v>20</v>
+      </c>
+      <c r="G10" s="9">
+        <v>40</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="9">
+        <f>F11-8/100*F11</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F11" s="9">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9">
+        <f>F11+8/100*F11</f>
+        <v>10.8</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5">
+        <f>F12-8/100*F12</f>
+        <v>0.92</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <f>F12+8/100*F12</f>
+        <v>1.08</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="37"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="5">
+        <v>760</v>
+      </c>
+      <c r="F18" s="5">
+        <v>800</v>
+      </c>
+      <c r="G18" s="5">
+        <v>840</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="J21" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="34"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="37"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="44"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="44"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="19">
+        <f>E10/10</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="19">
+        <f>F10/10</f>
+        <v>2</v>
+      </c>
+      <c r="G24" s="19">
+        <f>G10/10</f>
+        <v>4</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="18">
+        <f>((E9-G18*10^-3)/(G12*10^3)-G25*10^-6)*10^3</f>
+        <v>1.9086956521739131</v>
+      </c>
+      <c r="M24" s="18">
+        <f>((F9-F18*10^-3)/(F12*10^3)-F25*10^-6)*10^3</f>
+        <v>2.4200000000000004</v>
+      </c>
+      <c r="N24" s="18">
+        <f>((G9-E18*10^-3)/(E12*10^3)-E25*10^-6)*10^3</f>
+        <v>5.081803542673109</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="19">
+        <f>(E18*10^-3/(G11*10^3))*10^6</f>
+        <v>70.370370370370367</v>
+      </c>
+      <c r="F25" s="19">
+        <f>(F18*10^-3/(F11*10^3))*10^6</f>
+        <v>80</v>
+      </c>
+      <c r="G25" s="19">
+        <f>(G18*10^-3/(E11*10^3))*10^6</f>
+        <v>91.304347826086953</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="20">
+        <f>E10/N24</f>
+        <v>1.9678053108562008</v>
+      </c>
+      <c r="M25" s="20">
+        <f>F10/M24</f>
+        <v>8.2644628099173545</v>
+      </c>
+      <c r="N25" s="20">
+        <f>G10/L24</f>
+        <v>20.956719817767652</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="19">
+        <f>E24+E25*10^-3</f>
+        <v>1.0703703703703704</v>
+      </c>
+      <c r="F26" s="19">
+        <f>F24+F25*10^-3</f>
+        <v>2.08</v>
+      </c>
+      <c r="G26" s="19">
+        <f>G24+G25*10^-3</f>
+        <v>4.0913043478260871</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="20">
+        <f>(E9-G18*10^-3)/G26</f>
+        <v>0.52794899043570676</v>
+      </c>
+      <c r="F27" s="20">
+        <f>(F9-F18*10^-3)/F26</f>
+        <v>1.2019230769230769</v>
+      </c>
+      <c r="G27" s="20">
+        <f>(G9-E18*10^-3)/E26</f>
+        <v>4.428373702422145</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="J30" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="47"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="48"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="50"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="50"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="53"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="53"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="51"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="53"/>
+    </row>
+    <row r="35" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="56"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="51"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="53"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="56"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="C31:H39"/>
+    <mergeCell ref="J31:O35"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="D3:N3"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C7:C8"/>
@@ -10308,7 +12824,6 @@
     <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>